<commit_message>
All three schedules updated
</commit_message>
<xml_diff>
--- a/schedule/advisement/advisement.xlsx
+++ b/schedule/advisement/advisement.xlsx
@@ -5,17 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moberme\Documents\cslaee.com\schedule\advisement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moberme\Desktop\web\schedule\advisement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150"/>
   </bookViews>
   <sheets>
-    <sheet name="F18" sheetId="4" r:id="rId1"/>
-    <sheet name="S18" sheetId="3" r:id="rId2"/>
-    <sheet name="F17" sheetId="2" r:id="rId3"/>
-    <sheet name="S17" sheetId="1" r:id="rId4"/>
+    <sheet name="S19" sheetId="5" r:id="rId1"/>
+    <sheet name="F18" sheetId="4" r:id="rId2"/>
+    <sheet name="S18" sheetId="3" r:id="rId3"/>
+    <sheet name="F17" sheetId="2" r:id="rId4"/>
+    <sheet name="S17" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>Prof Fred Daneshgaran</t>
   </si>
@@ -168,6 +169,21 @@
   </si>
   <si>
     <t>Monday/Thursday 5:00-6:00PM</t>
+  </si>
+  <si>
+    <t>SPRING 2019 Advisement Hours</t>
+  </si>
+  <si>
+    <t>Effective Jan 22nd 2019</t>
+  </si>
+  <si>
+    <t>To be determined</t>
+  </si>
+  <si>
+    <t>Tuesday/Thursday 3:00-5:00PM</t>
+  </si>
+  <si>
+    <t>Monday/Wednesday 625-725PM</t>
   </si>
 </sst>
 </file>
@@ -525,7 +541,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -535,20 +553,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+    </row>
     <row r="5" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
@@ -556,71 +576,73 @@
     </row>
     <row r="6" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="A8" s="6"/>
+    </row>
+    <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="10" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="14" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="A20" s="6"/>
     </row>
     <row r="21" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
@@ -741,9 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A126"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -753,22 +773,20 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-    </row>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
@@ -776,30 +794,28 @@
     </row>
     <row r="6" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -807,22 +823,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
+    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -830,9 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-    </row>
+    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>7</v>
@@ -840,7 +852,7 @@
     </row>
     <row r="20" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -965,11 +977,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A126"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,64 +991,68 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="A4" s="6"/>
     </row>
     <row r="5" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1045,30 +1060,30 @@
     </row>
     <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1188,6 +1203,229 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:A126"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="99.85546875" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+    </row>
+    <row r="6" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="23" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A27"/>
   <sheetViews>

</xml_diff>